<commit_message>
Removed testing line from data_exclude
</commit_message>
<xml_diff>
--- a/data/data_selection/data_exclude.xlsx
+++ b/data/data_selection/data_exclude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB33691-65AF-EE4F-9977-3C5699A87A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F6C765-3F9E-A541-B282-0488F526FDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{849F44EE-864A-2941-BE9D-07802BBF1516}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Species</t>
   </si>
@@ -54,18 +54,6 @@
   </si>
   <si>
     <t># Make sure that the cell format is text rather than Excel's date format</t>
-  </si>
-  <si>
-    <t>ch4</t>
-  </si>
-  <si>
-    <t>GAGE</t>
-  </si>
-  <si>
-    <t>1990-01-01 00:00</t>
-  </si>
-  <si>
-    <t>1991-01-01 00:00</t>
   </si>
   <si>
     <t># Mole fraction data during the ranges in this worksheet will be excluded</t>
@@ -421,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2E2565-FF09-8844-8E81-909A9E1AB26D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,7 +423,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -460,20 +448,6 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP: Started a module to run processing. Added info to release schedule
</commit_message>
<xml_diff>
--- a/data/data_selection/data_exclude.xlsx
+++ b/data/data_selection/data_exclude.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F6C765-3F9E-A541-B282-0488F526FDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D35935-3203-F44A-8D46-6F9192E9AF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{849F44EE-864A-2941-BE9D-07802BBF1516}"/>
+    <workbookView xWindow="9740" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{849F44EE-864A-2941-BE9D-07802BBF1516}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
+    <sheet name="THD" sheetId="3" r:id="rId2"/>
+    <sheet name="MHD" sheetId="4" r:id="rId3"/>
+    <sheet name="CMN" sheetId="5" r:id="rId4"/>
+    <sheet name="GSN" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>Species</t>
   </si>
@@ -57,6 +61,57 @@
   </si>
   <si>
     <t># Mole fraction data during the ranges in this worksheet will be excluded</t>
+  </si>
+  <si>
+    <t>hfc-32</t>
+  </si>
+  <si>
+    <t>GCMS-Medusa</t>
+  </si>
+  <si>
+    <t>2014-03-01 00:00</t>
+  </si>
+  <si>
+    <t>2015-08-31 00:00</t>
+  </si>
+  <si>
+    <t>hfc-125</t>
+  </si>
+  <si>
+    <t>ch2cl2</t>
+  </si>
+  <si>
+    <t>2011-05-01 00:00</t>
+  </si>
+  <si>
+    <t>2017-04-01 00:00</t>
+  </si>
+  <si>
+    <t>hfc-236fa</t>
+  </si>
+  <si>
+    <t>1970-01-01 00:00</t>
+  </si>
+  <si>
+    <t>2014-05-01 00:00</t>
+  </si>
+  <si>
+    <t>cfc-114</t>
+  </si>
+  <si>
+    <t>cfc-115</t>
+  </si>
+  <si>
+    <t>2006-01-01 00:00</t>
+  </si>
+  <si>
+    <t>2008-01-01 00:00</t>
+  </si>
+  <si>
+    <t>ch3br</t>
+  </si>
+  <si>
+    <t>2007-12-31 00:00</t>
   </si>
 </sst>
 </file>
@@ -411,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2E2565-FF09-8844-8E81-909A9E1AB26D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -453,4 +508,301 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0E551D-3078-234D-AE1D-6BA1BE098447}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90822AB9-DFAF-A248-A862-C81247904CD1}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A07B53-7B4A-7F45-9B4A-35A2B2F763FB}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CF8359-ADE1-CD4B-B555-BB6E08340988}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added data combination information for all sites/species. Mostly a guess by me, and will need checking
</commit_message>
<xml_diff>
--- a/data/data_selection/data_exclude.xlsx
+++ b/data/data_selection/data_exclude.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F4852-0053-FA49-BA5C-54A6D9442204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD98894D-B54C-0F4B-82FE-691BA81A2CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13320" yWindow="760" windowWidth="16380" windowHeight="17440" xr2:uid="{849F44EE-864A-2941-BE9D-07802BBF1516}"/>
+    <workbookView xWindow="13320" yWindow="760" windowWidth="16380" windowHeight="17440" activeTab="3" xr2:uid="{849F44EE-864A-2941-BE9D-07802BBF1516}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
@@ -266,19 +266,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -665,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2E2565-FF09-8844-8E81-909A9E1AB26D}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -940,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A07B53-7B4A-7F45-9B4A-35A2B2F763FB}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>